<commit_message>
feat(env-prepare): support judge os
</commit_message>
<xml_diff>
--- a/env-prepare/script-dev-plan.xlsx
+++ b/env-prepare/script-dev-plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/heaven/Workspaces/hz-9_workspace/collection-space/env-prepare/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9DE16F7-A9EB-4945-9ADB-1498938B8CCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E881F81-DC90-504A-822C-8A8BB95B51C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-3840" yWindow="-21600" windowWidth="38400" windowHeight="21600" xr2:uid="{CA7A8425-824C-9845-86D0-43A88A5B878A}"/>
   </bookViews>
@@ -278,38 +278,17 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -318,25 +297,37 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -677,88 +668,88 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H6" sqref="H6:I6"/>
+      <selection pane="topRight" activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="30" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="30.83203125" customWidth="1"/>
-    <col min="2" max="2" width="12.83203125" style="12" customWidth="1"/>
-    <col min="3" max="3" width="12.83203125" style="7" customWidth="1"/>
-    <col min="4" max="4" width="12.83203125" style="8" customWidth="1"/>
-    <col min="5" max="6" width="12.83203125" style="7" customWidth="1"/>
-    <col min="7" max="7" width="12.83203125" style="8" customWidth="1"/>
-    <col min="8" max="9" width="12.83203125" style="7" customWidth="1"/>
-    <col min="10" max="10" width="12.83203125" style="16" customWidth="1"/>
+    <col min="2" max="2" width="12.83203125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="12.83203125" customWidth="1"/>
+    <col min="4" max="4" width="12.83203125" style="3" customWidth="1"/>
+    <col min="5" max="6" width="12.83203125" customWidth="1"/>
+    <col min="7" max="7" width="12.83203125" style="3" customWidth="1"/>
+    <col min="8" max="9" width="12.83203125" customWidth="1"/>
+    <col min="10" max="10" width="12.83203125" style="7" customWidth="1"/>
     <col min="11" max="45" width="20.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="3" customFormat="1" ht="30" customHeight="1">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:10" s="2" customFormat="1" ht="30" customHeight="1">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="13"/>
-    </row>
-    <row r="2" spans="1:10" s="3" customFormat="1" ht="30" customHeight="1">
-      <c r="A2" s="1"/>
-      <c r="B2" s="10" t="s">
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="16"/>
+    </row>
+    <row r="2" spans="1:10" s="2" customFormat="1" ht="30" customHeight="1">
+      <c r="A2" s="11"/>
+      <c r="B2" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5" t="s">
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5" t="s">
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="5"/>
-      <c r="J2" s="14"/>
-    </row>
-    <row r="3" spans="1:10" s="3" customFormat="1" ht="30" customHeight="1">
-      <c r="A3" s="2"/>
-      <c r="B3" s="11" t="s">
+      <c r="I2" s="11"/>
+      <c r="J2" s="13"/>
+    </row>
+    <row r="3" spans="1:10" s="2" customFormat="1" ht="30" customHeight="1">
+      <c r="A3" s="1"/>
+      <c r="B3" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="H3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="I3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="J3" s="6" t="s">
+      <c r="J3" s="1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="30" customHeight="1">
-      <c r="H4" s="19" t="s">
+      <c r="B4" s="10" t="s">
         <v>24</v>
       </c>
     </row>
@@ -766,22 +757,22 @@
       <c r="A5" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5" s="18" t="s">
+      <c r="B5" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="F5" s="18" t="s">
+      <c r="F5" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="H5" s="18" t="s">
+      <c r="H5" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="I5" s="18" t="s">
+      <c r="I5" s="9" t="s">
         <v>23</v>
       </c>
     </row>
@@ -789,22 +780,22 @@
       <c r="A6" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="E6" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="F6" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="H6" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="I6" s="17" t="s">
+      <c r="B6" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="I6" s="8" t="s">
         <v>22</v>
       </c>
     </row>
@@ -817,22 +808,22 @@
       <c r="A8" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="E8" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="F8" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="H8" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="I8" s="17" t="s">
+      <c r="B8" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="I8" s="8" t="s">
         <v>22</v>
       </c>
     </row>
@@ -855,22 +846,22 @@
       <c r="A12" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="C12" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="E12" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="F12" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="H12" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="I12" s="17" t="s">
+      <c r="B12" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H12" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="I12" s="8" t="s">
         <v>22</v>
       </c>
     </row>
@@ -904,77 +895,77 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="30" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="30.83203125" customWidth="1"/>
-    <col min="2" max="2" width="12.83203125" style="12" customWidth="1"/>
-    <col min="3" max="3" width="12.83203125" style="7" customWidth="1"/>
-    <col min="4" max="4" width="12.83203125" style="8" customWidth="1"/>
-    <col min="5" max="6" width="12.83203125" style="7" customWidth="1"/>
-    <col min="7" max="7" width="12.83203125" style="8" customWidth="1"/>
-    <col min="8" max="9" width="12.83203125" style="7" customWidth="1"/>
-    <col min="10" max="10" width="12.83203125" style="16" customWidth="1"/>
+    <col min="2" max="2" width="12.83203125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="12.83203125" customWidth="1"/>
+    <col min="4" max="4" width="12.83203125" style="3" customWidth="1"/>
+    <col min="5" max="6" width="12.83203125" customWidth="1"/>
+    <col min="7" max="7" width="12.83203125" style="3" customWidth="1"/>
+    <col min="8" max="9" width="12.83203125" customWidth="1"/>
+    <col min="10" max="10" width="12.83203125" style="7" customWidth="1"/>
     <col min="11" max="45" width="20.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="3" customFormat="1" ht="30" customHeight="1">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:10" s="2" customFormat="1" ht="30" customHeight="1">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="13"/>
-    </row>
-    <row r="2" spans="1:10" s="3" customFormat="1" ht="30" customHeight="1">
-      <c r="A2" s="1"/>
-      <c r="B2" s="10" t="s">
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="16"/>
+    </row>
+    <row r="2" spans="1:10" s="2" customFormat="1" ht="30" customHeight="1">
+      <c r="A2" s="11"/>
+      <c r="B2" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5" t="s">
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5" t="s">
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="5"/>
-      <c r="J2" s="14"/>
-    </row>
-    <row r="3" spans="1:10" s="3" customFormat="1" ht="30" customHeight="1">
-      <c r="A3" s="2"/>
-      <c r="B3" s="11" t="s">
+      <c r="I2" s="11"/>
+      <c r="J2" s="13"/>
+    </row>
+    <row r="3" spans="1:10" s="2" customFormat="1" ht="30" customHeight="1">
+      <c r="A3" s="1"/>
+      <c r="B3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="H3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="I3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="J3" s="15" t="s">
+      <c r="J3" s="6" t="s">
         <v>11</v>
       </c>
     </row>
@@ -997,10 +988,10 @@
       <c r="A8" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="17" t="s">
+      <c r="E8" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="F8" s="17" t="s">
+      <c r="F8" s="8" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1023,10 +1014,10 @@
       <c r="A12" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="17" t="s">
+      <c r="E12" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="F12" s="17" t="s">
+      <c r="F12" s="8" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feat(env-prepare): support `Debian` `Fedora` `Alibaba Cloud Linux` `Red Hat`
</commit_message>
<xml_diff>
--- a/env-prepare/script-dev-plan.xlsx
+++ b/env-prepare/script-dev-plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/heaven/Workspaces/hz-9_workspace/collection-space/env-prepare/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E881F81-DC90-504A-822C-8A8BB95B51C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3179F43-655B-614F-8626-283EE2F0A20C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-3840" yWindow="-21600" windowWidth="38400" windowHeight="21600" xr2:uid="{CA7A8425-824C-9845-86D0-43A88A5B878A}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="37">
   <si>
     <t>Script Name</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -134,6 +134,53 @@
   </si>
   <si>
     <t>Error</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Debian</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>11.9 (x64)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>12.2 (x64)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fedora</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>40 (x64)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Alibaba Cloud Linux</t>
+  </si>
+  <si>
+    <t>3.2.104 (x64)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Red Hat</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>8.5 (x64)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>9.0  (x64)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>p7Zip</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>7zip</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -183,7 +230,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -214,8 +261,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -272,13 +325,81 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -306,18 +427,15 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -329,6 +447,72 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -664,219 +848,595 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD77C587-048C-7548-B4DE-058EFEE3C19D}">
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:AB18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="K14" sqref="K14"/>
+      <selection pane="topRight" activeCell="B5" sqref="B5:X5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="30" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="16.83203125" defaultRowHeight="30" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="30.83203125" customWidth="1"/>
-    <col min="2" max="2" width="12.83203125" style="5" customWidth="1"/>
-    <col min="3" max="3" width="12.83203125" customWidth="1"/>
-    <col min="4" max="4" width="12.83203125" style="3" customWidth="1"/>
-    <col min="5" max="6" width="12.83203125" customWidth="1"/>
-    <col min="7" max="7" width="12.83203125" style="3" customWidth="1"/>
-    <col min="8" max="9" width="12.83203125" customWidth="1"/>
-    <col min="10" max="10" width="12.83203125" style="7" customWidth="1"/>
-    <col min="11" max="45" width="20.83203125" customWidth="1"/>
+    <col min="1" max="3" width="16.83203125" style="19"/>
+    <col min="4" max="4" width="16.83203125" style="22"/>
+    <col min="5" max="6" width="16.83203125" style="19"/>
+    <col min="7" max="7" width="16.83203125" style="22"/>
+    <col min="8" max="9" width="16.83203125" style="19"/>
+    <col min="10" max="10" width="16.83203125" style="22"/>
+    <col min="11" max="16384" width="16.83203125" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1" ht="30" customHeight="1">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:28" s="17" customFormat="1" ht="30" customHeight="1">
+      <c r="A1" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="16"/>
-    </row>
-    <row r="2" spans="1:10" s="2" customFormat="1" ht="30" customHeight="1">
-      <c r="A2" s="11"/>
-      <c r="B2" s="12" t="s">
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="L1" s="23"/>
+      <c r="M1" s="23"/>
+      <c r="N1" s="23"/>
+      <c r="O1" s="23"/>
+      <c r="P1" s="24"/>
+      <c r="Q1" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="R1" s="23"/>
+      <c r="S1" s="24"/>
+      <c r="T1" s="32" t="s">
+        <v>30</v>
+      </c>
+      <c r="U1" s="23"/>
+      <c r="V1" s="24"/>
+      <c r="W1" s="32" t="s">
+        <v>32</v>
+      </c>
+      <c r="X1" s="23"/>
+      <c r="Y1" s="23"/>
+      <c r="Z1" s="23"/>
+      <c r="AA1" s="23"/>
+      <c r="AB1" s="24"/>
+    </row>
+    <row r="2" spans="1:28" s="17" customFormat="1" ht="30" customHeight="1">
+      <c r="A2" s="34"/>
+      <c r="B2" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11" t="s">
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11" t="s">
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="11"/>
-      <c r="J2" s="13"/>
-    </row>
-    <row r="3" spans="1:10" s="2" customFormat="1" ht="30" customHeight="1">
-      <c r="A3" s="1"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="12"/>
+      <c r="K2" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="L2" s="16"/>
+      <c r="M2" s="16"/>
+      <c r="N2" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="O2" s="16"/>
+      <c r="P2" s="12"/>
+      <c r="Q2" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="R2" s="16"/>
+      <c r="S2" s="12"/>
+      <c r="T2" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="U2" s="16"/>
+      <c r="V2" s="12"/>
+      <c r="W2" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="X2" s="16"/>
+      <c r="Y2" s="16"/>
+      <c r="Z2" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="AA2" s="16"/>
+      <c r="AB2" s="12"/>
+    </row>
+    <row r="3" spans="1:28" s="17" customFormat="1" ht="30" customHeight="1">
+      <c r="A3" s="35"/>
       <c r="B3" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G3" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H3" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="I3" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="J3" s="6" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" ht="30" customHeight="1">
-      <c r="B4" s="10" t="s">
+      <c r="K3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="L3" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="M3" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="N3" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="O3" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="P3" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="R3" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="S3" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="T3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="U3" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="V3" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="W3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="X3" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="Y3" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="Z3" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="AA3" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="AB3" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" ht="30" customHeight="1">
+      <c r="A4" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="I4" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="J4" s="7"/>
+      <c r="K4" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="L4" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="N4" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="O4" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="P4" s="9"/>
+      <c r="Q4" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="R4" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="S4" s="9"/>
+      <c r="T4" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="U4" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="V4" s="9"/>
+      <c r="W4" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="X4" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="Z4" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="AA4" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="AB4" s="9"/>
+    </row>
+    <row r="5" spans="1:28" ht="30" customHeight="1">
+      <c r="A5" s="36" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="N5" s="5"/>
+      <c r="P5" s="5"/>
+      <c r="R5" s="5"/>
+      <c r="T5" s="5"/>
+      <c r="V5" s="5"/>
+      <c r="X5" s="5"/>
+      <c r="Z5" s="20"/>
+      <c r="AA5" s="20"/>
+      <c r="AB5" s="9"/>
+    </row>
+    <row r="6" spans="1:28" ht="30" customHeight="1">
+      <c r="A6" s="36" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="H6" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="I6" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="J6" s="7"/>
+      <c r="K6" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="L6" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="N6" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="O6" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="P6" s="9"/>
+      <c r="Q6" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="R6" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="S6" s="9"/>
+      <c r="T6" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="U6" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="V6" s="9"/>
+      <c r="W6" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="X6" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="Z6" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="AA6" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="AB6" s="9"/>
+    </row>
+    <row r="7" spans="1:28" ht="30" customHeight="1">
+      <c r="A7" s="36" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="5"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="5"/>
+      <c r="P7" s="9"/>
+      <c r="Q7" s="5"/>
+      <c r="S7" s="9"/>
+      <c r="T7" s="5"/>
+      <c r="V7" s="9"/>
+      <c r="W7" s="5"/>
+      <c r="AB7" s="9"/>
+    </row>
+    <row r="8" spans="1:28" ht="30" customHeight="1">
+      <c r="A8" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="H8" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="I8" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="J8" s="7"/>
+      <c r="K8" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="L8" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="N8" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="O8" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="P8" s="9"/>
+      <c r="Q8" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="R8" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="S8" s="9"/>
+      <c r="T8" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="U8" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="V8" s="9"/>
+      <c r="W8" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="X8" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="Z8" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="AA8" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="AB8" s="9"/>
+    </row>
+    <row r="9" spans="1:28" ht="30" customHeight="1">
+      <c r="A9" s="36" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="5"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="5"/>
+      <c r="P9" s="9"/>
+      <c r="Q9" s="5"/>
+      <c r="S9" s="9"/>
+      <c r="T9" s="5"/>
+      <c r="V9" s="9"/>
+      <c r="W9" s="5"/>
+      <c r="AB9" s="9"/>
+    </row>
+    <row r="10" spans="1:28" ht="30" customHeight="1">
+      <c r="A10" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="5"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="5"/>
+      <c r="P10" s="9"/>
+      <c r="Q10" s="5"/>
+      <c r="S10" s="9"/>
+      <c r="T10" s="5"/>
+      <c r="V10" s="9"/>
+      <c r="W10" s="5"/>
+      <c r="AB10" s="9"/>
+    </row>
+    <row r="11" spans="1:28" ht="30" customHeight="1">
+      <c r="A11" s="36" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="5"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="5"/>
+      <c r="P11" s="9"/>
+      <c r="Q11" s="5"/>
+      <c r="S11" s="9"/>
+      <c r="T11" s="5"/>
+      <c r="V11" s="9"/>
+      <c r="W11" s="5"/>
+      <c r="AB11" s="9"/>
+    </row>
+    <row r="12" spans="1:28" ht="30" customHeight="1">
+      <c r="A12" s="36" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="F12" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="H12" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="I12" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="J12" s="7"/>
+      <c r="K12" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="L12" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="N12" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="O12" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="P12" s="9"/>
+      <c r="Q12" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="R12" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="S12" s="9"/>
+      <c r="T12" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="U12" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="V12" s="9"/>
+      <c r="W12" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="X12" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="Z12" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="AA12" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="AB12" s="9"/>
+    </row>
+    <row r="13" spans="1:28" ht="30" customHeight="1">
+      <c r="A13" s="37" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="25"/>
+      <c r="C13" s="26"/>
+      <c r="D13" s="27"/>
+      <c r="E13" s="26"/>
+      <c r="F13" s="26"/>
+      <c r="G13" s="27"/>
+      <c r="H13" s="26"/>
+      <c r="I13" s="26"/>
+      <c r="J13" s="31"/>
+      <c r="K13" s="25"/>
+      <c r="L13" s="26"/>
+      <c r="M13" s="26"/>
+      <c r="N13" s="26"/>
+      <c r="O13" s="26"/>
+      <c r="P13" s="28"/>
+      <c r="Q13" s="25"/>
+      <c r="R13" s="26"/>
+      <c r="S13" s="28"/>
+      <c r="T13" s="25"/>
+      <c r="U13" s="26"/>
+      <c r="V13" s="28"/>
+      <c r="W13" s="25"/>
+      <c r="X13" s="26"/>
+      <c r="Y13" s="26"/>
+      <c r="Z13" s="26"/>
+      <c r="AA13" s="26"/>
+      <c r="AB13" s="28"/>
+    </row>
+    <row r="18" spans="2:4" ht="30" customHeight="1">
+      <c r="B18" s="29" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" ht="30" customHeight="1">
-      <c r="A5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5" s="9" t="s">
+      <c r="C18" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="F5" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="H5" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="I5" s="9" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="30" customHeight="1">
-      <c r="A6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="H6" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="I6" s="8" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="30" customHeight="1">
-      <c r="A7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="30" customHeight="1">
-      <c r="A8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="F8" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="H8" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="I8" s="8" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="30" customHeight="1">
-      <c r="A9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="30" customHeight="1">
-      <c r="A10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="30" customHeight="1">
-      <c r="A11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="30" customHeight="1">
-      <c r="A12" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="E12" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="F12" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="H12" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="I12" s="8" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="30" customHeight="1">
-      <c r="A13" t="s">
-        <v>8</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="15">
+    <mergeCell ref="W1:AB1"/>
+    <mergeCell ref="W2:Y2"/>
+    <mergeCell ref="Z2:AB2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="E2:G2"/>
     <mergeCell ref="H2:J2"/>
     <mergeCell ref="B1:J1"/>
+    <mergeCell ref="K2:M2"/>
+    <mergeCell ref="N2:P2"/>
+    <mergeCell ref="K1:P1"/>
+    <mergeCell ref="Q2:S2"/>
+    <mergeCell ref="T2:V2"/>
+    <mergeCell ref="Q1:S1"/>
+    <mergeCell ref="T1:V1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -909,21 +1469,21 @@
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="16"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="15"/>
     </row>
     <row r="2" spans="1:10" s="2" customFormat="1" ht="30" customHeight="1">
       <c r="A2" s="11"/>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="10" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="11"/>
@@ -937,7 +1497,7 @@
         <v>16</v>
       </c>
       <c r="I2" s="11"/>
-      <c r="J2" s="13"/>
+      <c r="J2" s="12"/>
     </row>
     <row r="3" spans="1:10" s="2" customFormat="1" ht="30" customHeight="1">
       <c r="A3" s="1"/>

</xml_diff>